<commit_message>
Ahora se regresa el nombr del distribuidor y se actualizaron los ejemplos de distribuidor
</commit_message>
<xml_diff>
--- a/distribuidores_ejemplo.xlsx
+++ b/distribuidores_ejemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sistema\Documentos\GitHub\Xpatl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2555E64-ED6E-46D7-90FD-59EE283FF2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B861F69-281A-4044-870E-2F6F171F2490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11565" yWindow="4230" windowWidth="12330" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22305" yWindow="4050" windowWidth="12330" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Nombre</t>
   </si>
@@ -28,16 +28,88 @@
     <t>Descuento</t>
   </si>
   <si>
-    <t>Distribuidora Perez</t>
-  </si>
-  <si>
-    <t>Distribuidora Luz</t>
-  </si>
-  <si>
-    <t>ITECMI</t>
-  </si>
-  <si>
-    <t>Distribuidor 200</t>
+    <t>ANA KARINA GARCIA.</t>
+  </si>
+  <si>
+    <t>BERTHA MARQUEZ.</t>
+  </si>
+  <si>
+    <t>DOMITILA VILLASEÑOR.</t>
+  </si>
+  <si>
+    <t>ERNESTINA VILLA.</t>
+  </si>
+  <si>
+    <t>GRACIA LIMON.</t>
+  </si>
+  <si>
+    <t>GUADALUPE SOLTERO.</t>
+  </si>
+  <si>
+    <t>HILARIA VILLASEÑOR.</t>
+  </si>
+  <si>
+    <t>LILIA ZARAGOZA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOURDES GOMEZ. </t>
+  </si>
+  <si>
+    <t>MARTHA ZARAGOZA/ESC DERMOCOS</t>
+  </si>
+  <si>
+    <t>MIRNA SAMANIEGO.</t>
+  </si>
+  <si>
+    <t>ROSARIO ORUETA.</t>
+  </si>
+  <si>
+    <t>TERESA QUERETARO.</t>
+  </si>
+  <si>
+    <t>VIANEY SELENE BELTRAN LOPEZ.</t>
+  </si>
+  <si>
+    <t>MARIO CASTRO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VICTORIA RUIZ. </t>
+  </si>
+  <si>
+    <t>ANA CECILIA CAMPECHE.</t>
+  </si>
+  <si>
+    <t>EVELYN SCHIDECK</t>
+  </si>
+  <si>
+    <t>GRACIELA CEBALLOS/INSTITUTO CIENCIAS COSMETICAS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HECTOR OCTAVIO. </t>
+  </si>
+  <si>
+    <t>ADRIANA LEON.</t>
+  </si>
+  <si>
+    <t>LUIS MIGUEL PEREGRINA.</t>
+  </si>
+  <si>
+    <t>MARICARMEN CONTRERAS.</t>
+  </si>
+  <si>
+    <t>ROCIO SIERRA.</t>
+  </si>
+  <si>
+    <t>ELVIRA SERRANO.</t>
+  </si>
+  <si>
+    <t>DIANA LETICIA OJEDA OJEDA.</t>
+  </si>
+  <si>
+    <t>MIGUEL ANGEL GARCIA ARELLANO.</t>
+  </si>
+  <si>
+    <t>JESICA ADRIANA LOPEZ TORRES (ZAZIL)</t>
   </si>
 </sst>
 </file>
@@ -882,7 +954,7 @@
   <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -911,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -919,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,7 +999,199 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>99</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>45</v>
       </c>
     </row>
     <row r="224" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
La ruta de obtener los distribuidores
Ahora la ruta acepta GET y POST. POST acepta filtros para la pantalla de gestíon de distribuidores
</commit_message>
<xml_diff>
--- a/distribuidores_ejemplo.xlsx
+++ b/distribuidores_ejemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sistema\Documentos\GitHub\Xpatl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B861F69-281A-4044-870E-2F6F171F2490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E72E50B-06FD-4A3A-BF05-8181B74B3F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22305" yWindow="4050" windowWidth="12330" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="A30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>